<commit_message>
Kraftwerksgrafik in Visualisierung eingebaut
</commit_message>
<xml_diff>
--- a/data/Knotentabelle.xlsx
+++ b/data/Knotentabelle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lars/Documents/MATLAB/Netzsimulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603C8D78-0DFA-B641-836C-C7C5C8879B4E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D45A759-EA52-C849-A78C-0C27673EF0C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16220" xr2:uid="{109839D1-D567-AA4B-87D7-F86B2B8F67E9}"/>
   </bookViews>
@@ -424,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660CDFC1-36C3-6D4A-97C5-40145D00575F}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="260" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -463,10 +463,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D2">
         <v>500</v>
@@ -484,7 +484,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3">
         <v>23</v>
@@ -508,7 +508,7 @@
         <v>47</v>
       </c>
       <c r="C4">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <v>700</v>
@@ -526,7 +526,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C5">
         <v>25</v>

</xml_diff>

<commit_message>
Tabellendaten aktualisiert für Testzwecke.
</commit_message>
<xml_diff>
--- a/data/Knotentabelle.xlsx
+++ b/data/Knotentabelle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lars/Documents/MATLAB/Netzsimulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881E003B-1162-0C4B-8280-454659B44DDB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E07765-89E5-734C-833C-43EB0A225F50}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16220" xr2:uid="{109839D1-D567-AA4B-87D7-F86B2B8F67E9}"/>
+    <workbookView xWindow="8380" yWindow="1060" windowWidth="28800" windowHeight="16240" xr2:uid="{109839D1-D567-AA4B-87D7-F86B2B8F67E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -425,7 +425,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="260" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -466,7 +466,7 @@
         <v>59</v>
       </c>
       <c r="C2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2">
         <v>500</v>
@@ -484,10 +484,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3">
         <v>1000</v>
@@ -505,10 +505,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C4">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4">
         <v>700</v>
@@ -526,7 +526,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C5">
         <v>25</v>
@@ -547,10 +547,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C6">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6">
         <v>1200</v>
@@ -568,7 +568,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C7">
         <v>29</v>
@@ -589,7 +589,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C8">
         <v>25</v>
@@ -610,10 +610,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C9">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>200</v>
@@ -631,10 +631,10 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C10">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>400</v>

</xml_diff>

<commit_message>
Kostendifferenzierung eingebaut, bessere Werte in Knotentabelle eingefügt
</commit_message>
<xml_diff>
--- a/data/Knotentabelle.xlsx
+++ b/data/Knotentabelle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lars/Documents/MATLAB/Netzsimulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863442DF-4026-B14D-93CA-4A0781744655}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBD7FC6-7384-1145-9FBB-4421642844D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16240" xr2:uid="{109839D1-D567-AA4B-87D7-F86B2B8F67E9}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16320" xr2:uid="{109839D1-D567-AA4B-87D7-F86B2B8F67E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -417,8 +417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660CDFC1-36C3-6D4A-97C5-40145D00575F}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="260" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -462,11 +462,11 @@
         <v>22</v>
       </c>
       <c r="D2">
-        <v>500</v>
+        <v>1000000</v>
       </c>
       <c r="E2">
-        <f>3*D2</f>
-        <v>1500</v>
+        <f xml:space="preserve"> (D2*12)/60+(D2/10000)*500000/20</f>
+        <v>2700000</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -483,11 +483,11 @@
         <v>22</v>
       </c>
       <c r="D3">
-        <v>1000</v>
+        <v>2000000</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E10" si="0">3*D3</f>
-        <v>3000</v>
+        <f t="shared" ref="E3:E10" si="0" xml:space="preserve"> (D3*12)/60+(D3/10000)*500000/20</f>
+        <v>5400000</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -504,11 +504,11 @@
         <v>22</v>
       </c>
       <c r="D4">
-        <v>700</v>
+        <v>700000</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>2100</v>
+        <v>1890000</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -525,11 +525,11 @@
         <v>25</v>
       </c>
       <c r="D5">
-        <v>300</v>
+        <v>300000</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>810000</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -546,11 +546,11 @@
         <v>27</v>
       </c>
       <c r="D6">
-        <v>1200</v>
+        <v>2000000</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>3600</v>
+        <v>5400000</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -567,11 +567,11 @@
         <v>29</v>
       </c>
       <c r="D7">
-        <v>100</v>
+        <v>100000</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>270000</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -588,11 +588,11 @@
         <v>25</v>
       </c>
       <c r="D8">
-        <v>1500</v>
+        <v>1500000</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>4500</v>
+        <v>4050000</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -609,11 +609,11 @@
         <v>30</v>
       </c>
       <c r="D9">
-        <v>200</v>
+        <v>750000</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>600</v>
+        <v>2025000</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -630,11 +630,11 @@
         <v>30</v>
       </c>
       <c r="D10">
-        <v>400</v>
+        <v>400000</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>1080000</v>
       </c>
       <c r="F10">
         <v>1</v>

</xml_diff>